<commit_message>
Add web crawler dashboard with target management and data extraction functionality
- Implemented Flask web application for managing scraping targets and initiating crawling.
- Added functionality to read and write targets from/to a CSV file.
- Developed a multi-threaded crawling process that extracts data and saves it to an Excel file.
- Created HTML template for user interface with progress tracking and download options.
- Included JavaScript for asynchronous updates and interactions with the backend.
- Added routes for adding, deleting targets, checking progress, and downloading results.
</commit_message>
<xml_diff>
--- a/alle_projekte.xlsx
+++ b/alle_projekte.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +425,355 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Website</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Projektname</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Haslehner</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Elementum Marchtrenk</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://www.haslehner.net/projekte/elementum-marchtrenk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Haslehner</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Silberweiß 25, Amstetten</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://www.haslehner.net/projekte/silberweiss-25-amstetten/</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Haslehner</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>rmg56 - Rotenmühlgasse 56, 1120 Wien</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>https://www.haslehner.net/projekte/rmg56-rotenmuehlgasse-56-1120-wien/</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Haslehner</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Ski &amp; Panorama Living - Saalbach-Hinterglemm</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>https://www.haslehner.net/projekte/ski-panorama-living-saalbach-hinterglemm/</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Haslehner</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Hüttelbergstraße 73, 1140 Wien</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>https://www.haslehner.net/projekte/huettelbergstrasse-73-1140-wien/</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Haslehner</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>W4 Wallern a.d.T.</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://www.haslehner.net/projekte/w4-wallern-adt/</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Haslehner</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Martinstraße 86, 1180 Wien</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>https://www.haslehner.net/projekte/martinstrasse-86-1180-wien/</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Haslehner</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Wohnen 4712 2.0 - Michaelnbach</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>https://www.haslehner.net/projekte/wohnen-4712-20-michaelnbach/</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Haslehner</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Moserstraße 25C, 5020 Salzburg</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>https://www.haslehner.net/projekte/moserstrasse-25c-5020-salzburg/</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Haslehner</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>München Stockdorf</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>https://www.haslehner.net/projekte/muenchen-stockdorf/</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Haslehner</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Conrad von Hötzendorf-Platz 3A, 2500 Baden</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>https://www.haslehner.net/projekte/conrad-von-hoetzendorf-platz-3a-2500-baden/</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Haslehner</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Käutzlgasse Salzburg</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>https://www.haslehner.net/projekte/kaeutzlgasse-salzburg/</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>OOEWohnbau</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Alkoven, Am Dorfplatz 2 - geförderte Mietwohnungen</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>https://ooewohnbau.at/immobiliensuche/details/alkoven-am-dorfplatz-gefoerderte-wohnungen</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>OOEWohnbau</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Andorf, Raaber Straße - 27 geförderte Miet- und Mietkaufwohnungen</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>https://ooewohnbau.at/immobiliensuche/details/wohnungen-andorf-gefoerderte-miet-mietkaufwohnungen</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>OOEWohnbau</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Ansfelden, Widistraße - Doppel- und Reihenhäuser / Eigentum ff und Miete mit Kaufoption ff</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>https://ooewohnbau.at/immobiliensuche/details/ansfelden-widistrasse-17-doppel-und-reihenhaeuser-/-eigentum-ff-und-miete-mit-kaufoption-ff</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>OOEWohnbau</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Bad Leonfelden, Hochstraße 3 - 15 geförderte Mietwohnungen mit Kaufoption</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>https://ooewohnbau.at/immobiliensuche/details/wohnungen-bad-leonfelden-hochstrasse-gefoerderte-mietkaufwohnungen</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>OOEWohnbau</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Grieskirchen, Keplerweg - 21 geförderte Eigentumswohnungen</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>https://ooewohnbau.at/immobiliensuche/details/eigentumswohnungen-in-grieskirchen-21-gefoerderte-eigentumswohnungen-in-grieskirchen</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>OOEWohnbau</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Hörsching, Brucknerplatz - Eigentum förderbar oder Miete mit Kaufoption</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>https://ooewohnbau.at/immobiliensuche/details/hoersching-brucknerplatz-28-gefoerderte-eigentumswohnungen</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>OOEWohnbau</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Hörsching, Brucknerplatz - Geschäftsfläche Eigentum oder Miete</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>https://ooewohnbau.at/immobiliensuche/details/geschaeftsflaeche-in-hoersching</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>